<commit_message>
Create sample with missing value.
</commit_message>
<xml_diff>
--- a/datasets/Online_Retail_1.xlsx
+++ b/datasets/Online_Retail_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ai2020\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\github.com\thachln\thachln.github.io.git\thachln.github.io\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115C499A-5C19-4EDF-8DE6-987292FA0B94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A73B36-46FC-4B56-A342-10B1674CD3AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>InvoiceNo</t>
   </si>
@@ -406,11 +406,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="A1:G7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -473,17 +471,17 @@
       <c r="A3" s="5">
         <v>536365</v>
       </c>
-      <c r="B3" s="6">
-        <v>71053</v>
+      <c r="B3" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3" s="7">
         <v>40513.351388888892</v>
       </c>
       <c r="E3">
-        <v>3.39</v>
+        <v>2.75</v>
       </c>
       <c r="F3" s="8">
         <v>17850</v>
@@ -497,20 +495,18 @@
         <v>536365</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="7">
         <v>40513.351388888892</v>
       </c>
       <c r="E4">
-        <v>2.75</v>
-      </c>
-      <c r="F4" s="8">
-        <v>17850</v>
-      </c>
+        <v>3.39</v>
+      </c>
+      <c r="F4" s="8"/>
       <c r="G4" t="s">
         <v>8</v>
       </c>
@@ -520,7 +516,7 @@
         <v>536365</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -542,45 +538,22 @@
       <c r="A6" s="5">
         <v>536365</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>11</v>
+      <c r="B6" s="6">
+        <v>22752</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D6" s="7">
         <v>40513.351388888892</v>
       </c>
       <c r="E6">
-        <v>3.39</v>
+        <v>7.65</v>
       </c>
       <c r="F6" s="8">
         <v>17850</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>536365</v>
-      </c>
-      <c r="B7" s="6">
-        <v>22752</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="7">
-        <v>40513.351388888892</v>
-      </c>
-      <c r="E7">
-        <v>7.65</v>
-      </c>
-      <c r="F7" s="8">
-        <v>17850</v>
-      </c>
-      <c r="G7" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>